<commit_message>
Update PR log from #23
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,36 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #24
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,36 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>24</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #25
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,36 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #26
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,6 +573,36 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #27
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,6 +603,36 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>27</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #29
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,6 +633,36 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>29</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>edit2 to main</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #30
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,6 +663,36 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>30</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Edit1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #31
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -693,6 +693,36 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>31</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Update index2.py</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>edit2 to main</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #33
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,6 +723,36 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Edit2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>edit2 to main</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #35
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,6 +753,36 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>35</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>time added</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #36
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -783,6 +783,36 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>36</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11:37</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #37
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,6 +813,36 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>37</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>latest timimg updated</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #39
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,6 +843,36 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>39</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>trying squashes</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #40
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,6 +873,36 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>40</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>change2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #41
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,6 +903,36 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>41</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>changed readme file</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #42
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -933,6 +933,36 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>42</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Update README.md</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #43
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,6 +963,36 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>43</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>small updates</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #44
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -993,6 +993,36 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>44</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #45
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1023,6 +1023,36 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>45</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>trying squash</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #46
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1053,6 +1053,36 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>46</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Edit1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #47
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1083,6 +1083,36 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>47</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>minor changes from edit2</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>edit2 to main</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #48
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,6 +1113,36 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>48</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Title_12:05</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #49
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1143,6 +1143,36 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>49</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>edit2 to main</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #50
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1143,6 +1143,36 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>50</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #51
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,6 +1173,36 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>51</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>try sq 2</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #52
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,6 +1203,36 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>52</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>okay added</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #53
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,6 +1233,36 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>53</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:26 added</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #54
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1263,6 +1263,36 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>54</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>math</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #55
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1293,6 +1293,36 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>55</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Edit1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #56
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1323,6 +1323,36 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>56</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>changes updated</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #57
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,6 +1173,36 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>57</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PR log from #58
</commit_message>
<xml_diff>
--- a/pull_reqs.xlsx
+++ b/pull_reqs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,6 +1203,36 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>58</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Update index.py</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>riyam2309</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>edit1 to main</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>